<commit_message>
q3 reporting and SU work
</commit_message>
<xml_diff>
--- a/Data/GEF Sampling/Litter Consolotaed ALL plots_2018.07.31.xlsx
+++ b/Data/GEF Sampling/Litter Consolotaed ALL plots_2018.07.31.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="179">
   <si>
     <t>Plot #</t>
   </si>
@@ -545,6 +545,24 @@
   </si>
   <si>
     <t>MV9</t>
+  </si>
+  <si>
+    <t>TCH-01</t>
+  </si>
+  <si>
+    <t>TCH-03</t>
+  </si>
+  <si>
+    <t>INT-01</t>
+  </si>
+  <si>
+    <t>INT-03</t>
+  </si>
+  <si>
+    <t>INT-07</t>
+  </si>
+  <si>
+    <t>from Tch_INT_Dry_Litter_2018.08.06_Cos.xlsx</t>
   </si>
 </sst>
 </file>
@@ -733,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -804,12 +822,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -829,7 +916,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="B9B9B9"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -9737,11 +9824,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10713,7 +10800,7 @@
         <v>6.0678867191493735E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>158</v>
       </c>
@@ -10730,7 +10817,7 @@
         <v>7.6161107955313889E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>159</v>
       </c>
@@ -10747,7 +10834,7 @@
         <v>5.9406781460328094E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>140</v>
       </c>
@@ -10757,7 +10844,7 @@
       </c>
       <c r="D67" s="21"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>141</v>
       </c>
@@ -10767,7 +10854,7 @@
       </c>
       <c r="D68" s="21"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>142</v>
       </c>
@@ -10784,7 +10871,7 @@
         <v>0.10267049781077495</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>143</v>
       </c>
@@ -10801,13 +10888,13 @@
         <v>7.8329920228991337E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>144</v>
       </c>
       <c r="D71" s="21"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>145</v>
       </c>
@@ -10824,7 +10911,7 @@
         <v>8.4116069899219992E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>146</v>
       </c>
@@ -10841,7 +10928,7 @@
         <v>8.7202148072870952E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>147</v>
       </c>
@@ -10858,7 +10945,7 @@
         <v>4.1016896870822821E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>148</v>
       </c>
@@ -10875,7 +10962,7 @@
         <v>0.11679040060167147</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>149</v>
       </c>
@@ -10885,7 +10972,7 @@
       </c>
       <c r="D76" s="21"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>150</v>
       </c>
@@ -10902,11 +10989,54 @@
         <v>8.9672490543907343E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="14"/>
       <c r="B78">
         <f>'Wet litter '!J79</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79">
+        <v>58.81</v>
+      </c>
+      <c r="E79" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="C80">
+        <v>110.56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C81">
+        <v>2768.91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82">
+        <v>2589.17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C83">
+        <v>3611.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>